<commit_message>
Fixed issue with part Ids
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -1346,7 +1346,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId16"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1415,7 +1415,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId18"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1475,7 +1475,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId20"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1529,7 +1529,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId22"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1674,7 +1674,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId24"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1728,7 +1728,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId26"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1782,7 +1782,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId28"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1842,7 +1842,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId30"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1890,7 +1890,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId32"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1949,7 +1949,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId34"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -1997,7 +1997,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:legacyDrawing r:id="rId2"/>
+  <x:legacyDrawing r:id="rId36"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Heights and widths no round to 6 decimal places.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Comments/AddingComments.xlsx
@@ -1188,166 +1188,41 @@
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
       <x:c r="E1" s="0" t="s"/>
-      <x:c r="F1" s="0" t="s"/>
       <x:c r="G1" s="0" t="s"/>
-      <x:c r="H1" s="0" t="s"/>
-      <x:c r="I1" s="0" t="s"/>
-      <x:c r="J1" s="0" t="s"/>
-      <x:c r="K1" s="0" t="s"/>
     </x:row>
     <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-      <x:c r="E2" s="0" t="s"/>
-      <x:c r="F2" s="0" t="s"/>
-      <x:c r="G2" s="0" t="s"/>
-      <x:c r="H2" s="0" t="s"/>
-      <x:c r="I2" s="0" t="s"/>
-      <x:c r="J2" s="0" t="s"/>
-      <x:c r="K2" s="0" t="s"/>
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
       <x:c r="E3" s="0" t="s"/>
-      <x:c r="F3" s="0" t="s"/>
       <x:c r="G3" s="0" t="s"/>
-      <x:c r="H3" s="0" t="s"/>
-      <x:c r="I3" s="0" t="s"/>
-      <x:c r="J3" s="0" t="s"/>
-      <x:c r="K3" s="0" t="s"/>
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-      <x:c r="E4" s="0" t="s"/>
-      <x:c r="F4" s="0" t="s"/>
-      <x:c r="G4" s="0" t="s"/>
-      <x:c r="H4" s="0" t="s"/>
-      <x:c r="I4" s="0" t="s"/>
-      <x:c r="J4" s="0" t="s"/>
-      <x:c r="K4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:11">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
-      <x:c r="F5" s="0" t="s"/>
-      <x:c r="G5" s="0" t="s"/>
-      <x:c r="H5" s="0" t="s"/>
-      <x:c r="I5" s="0" t="s"/>
-      <x:c r="J5" s="0" t="s"/>
-      <x:c r="K5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:11">
-      <x:c r="A6" s="0" t="s"/>
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
-      <x:c r="F6" s="0" t="s"/>
-      <x:c r="G6" s="0" t="s"/>
-      <x:c r="H6" s="0" t="s"/>
-      <x:c r="I6" s="0" t="s"/>
-      <x:c r="J6" s="0" t="s"/>
-      <x:c r="K6" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="5" spans="1:11"/>
+    <x:row r="6" spans="1:11"/>
     <x:row r="7" spans="1:11">
-      <x:c r="A7" s="0" t="s"/>
-      <x:c r="B7" s="0" t="s"/>
-      <x:c r="C7" s="0" t="s"/>
-      <x:c r="D7" s="0" t="s"/>
       <x:c r="E7" s="0" t="s"/>
-      <x:c r="F7" s="0" t="s"/>
-      <x:c r="G7" s="0" t="s"/>
-      <x:c r="H7" s="0" t="s"/>
-      <x:c r="I7" s="0" t="s"/>
-      <x:c r="J7" s="0" t="s"/>
-      <x:c r="K7" s="0" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:11">
-      <x:c r="A8" s="0" t="s"/>
-      <x:c r="B8" s="0" t="s"/>
-      <x:c r="C8" s="0" t="s"/>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
-      <x:c r="F8" s="0" t="s"/>
-      <x:c r="G8" s="0" t="s"/>
-      <x:c r="H8" s="0" t="s"/>
-      <x:c r="I8" s="0" t="s"/>
-      <x:c r="J8" s="0" t="s"/>
-      <x:c r="K8" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="8" spans="1:11"/>
     <x:row r="9" spans="1:11">
       <x:c r="A9" s="0" t="s"/>
-      <x:c r="B9" s="0" t="s"/>
-      <x:c r="C9" s="0" t="s"/>
       <x:c r="D9" s="0" t="s"/>
       <x:c r="E9" s="0" t="s"/>
       <x:c r="F9" s="0" t="s"/>
-      <x:c r="G9" s="0" t="s"/>
-      <x:c r="H9" s="0" t="s"/>
-      <x:c r="I9" s="0" t="s"/>
-      <x:c r="J9" s="0" t="s"/>
-      <x:c r="K9" s="0" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:11">
-      <x:c r="A10" s="0" t="s"/>
-      <x:c r="B10" s="0" t="s"/>
-      <x:c r="C10" s="0" t="s"/>
-      <x:c r="D10" s="0" t="s"/>
-      <x:c r="E10" s="0" t="s"/>
-      <x:c r="F10" s="0" t="s"/>
-      <x:c r="G10" s="0" t="s"/>
-      <x:c r="H10" s="0" t="s"/>
-      <x:c r="I10" s="0" t="s"/>
-      <x:c r="J10" s="0" t="s"/>
-      <x:c r="K10" s="0" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:11">
-      <x:c r="A11" s="0" t="s"/>
-      <x:c r="B11" s="0" t="s"/>
-      <x:c r="C11" s="0" t="s"/>
-      <x:c r="D11" s="0" t="s"/>
-      <x:c r="E11" s="0" t="s"/>
-      <x:c r="F11" s="0" t="s"/>
-      <x:c r="G11" s="0" t="s"/>
-      <x:c r="H11" s="0" t="s"/>
-      <x:c r="I11" s="0" t="s"/>
-      <x:c r="J11" s="0" t="s"/>
-      <x:c r="K11" s="0" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:11">
-      <x:c r="A12" s="0" t="s"/>
-      <x:c r="B12" s="0" t="s"/>
-      <x:c r="C12" s="0" t="s"/>
-      <x:c r="D12" s="0" t="s"/>
-      <x:c r="E12" s="0" t="s"/>
-      <x:c r="F12" s="0" t="s"/>
-      <x:c r="G12" s="0" t="s"/>
-      <x:c r="H12" s="0" t="s"/>
-      <x:c r="I12" s="0" t="s"/>
-      <x:c r="J12" s="0" t="s"/>
-      <x:c r="K12" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="10" spans="1:11"/>
+    <x:row r="11" spans="1:11"/>
+    <x:row r="12" spans="1:11"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1369,7 +1244,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="23.470625000000002" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="23.470625" style="0" customWidth="1"/>
     <x:col min="2" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -1377,46 +1252,19 @@
       <x:c r="A1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="A6" s="0" t="s"/>
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="A7" s="0" t="s"/>
-      <x:c r="B7" s="0" t="s"/>
-      <x:c r="C7" s="0" t="s"/>
-      <x:c r="D7" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="5" spans="1:4"/>
+    <x:row r="6" spans="1:4"/>
+    <x:row r="7" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1443,40 +1291,12 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-      <x:c r="E1" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="A6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="0" t="s"/>
-      <x:c r="C7" s="0" t="s"/>
-      <x:c r="D7" s="0" t="s"/>
-      <x:c r="E7" s="0" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="0" t="s"/>
-      <x:c r="C8" s="0" t="s"/>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="0" t="s"/>
-      <x:c r="C9" s="0" t="s"/>
-      <x:c r="D9" s="0" t="s"/>
-      <x:c r="E9" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="5" spans="1:5"/>
+    <x:row r="6" spans="1:5"/>
+    <x:row r="7" spans="1:5"/>
+    <x:row r="8" spans="1:5"/>
+    <x:row r="9" spans="1:5"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1501,36 +1321,13 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:4"/>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="4" spans="1:4"/>
+    <x:row r="5" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1557,125 +1354,24 @@
   <x:sheetData>
     <x:row r="1" spans="1:9">
       <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-      <x:c r="E1" s="0" t="s"/>
-      <x:c r="F1" s="0" t="s"/>
-      <x:c r="G1" s="0" t="s"/>
-      <x:c r="H1" s="0" t="s"/>
-      <x:c r="I1" s="0" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:9">
-      <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-      <x:c r="E2" s="0" t="s"/>
-      <x:c r="F2" s="0" t="s"/>
-      <x:c r="G2" s="0" t="s"/>
-      <x:c r="H2" s="0" t="s"/>
-      <x:c r="I2" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="2" spans="1:9"/>
     <x:row r="3" spans="1:9">
       <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
       <x:c r="D3" s="0" t="s"/>
       <x:c r="E3" s="0" t="s"/>
       <x:c r="F3" s="0" t="s"/>
-      <x:c r="G3" s="0" t="s"/>
-      <x:c r="H3" s="0" t="s"/>
-      <x:c r="I3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:9">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-      <x:c r="E4" s="0" t="s"/>
-      <x:c r="F4" s="0" t="s"/>
-      <x:c r="G4" s="0" t="s"/>
-      <x:c r="H4" s="0" t="s"/>
-      <x:c r="I4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:9">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
-      <x:c r="F5" s="0" t="s"/>
-      <x:c r="G5" s="0" t="s"/>
-      <x:c r="H5" s="0" t="s"/>
-      <x:c r="I5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:9">
-      <x:c r="A6" s="0" t="s"/>
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s"/>
-      <x:c r="F6" s="0" t="s"/>
-      <x:c r="G6" s="0" t="s"/>
-      <x:c r="H6" s="0" t="s"/>
-      <x:c r="I6" s="0" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:9">
-      <x:c r="A7" s="0" t="s"/>
-      <x:c r="B7" s="0" t="s"/>
-      <x:c r="C7" s="0" t="s"/>
-      <x:c r="D7" s="0" t="s"/>
-      <x:c r="E7" s="0" t="s"/>
-      <x:c r="F7" s="0" t="s"/>
-      <x:c r="G7" s="0" t="s"/>
-      <x:c r="H7" s="0" t="s"/>
-      <x:c r="I7" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="4" spans="1:9"/>
+    <x:row r="5" spans="1:9"/>
+    <x:row r="6" spans="1:9"/>
+    <x:row r="7" spans="1:9"/>
     <x:row r="8" spans="1:9">
       <x:c r="A8" s="0" t="s"/>
-      <x:c r="B8" s="0" t="s"/>
-      <x:c r="C8" s="0" t="s"/>
-      <x:c r="D8" s="0" t="s"/>
-      <x:c r="E8" s="0" t="s"/>
-      <x:c r="F8" s="0" t="s"/>
-      <x:c r="G8" s="0" t="s"/>
-      <x:c r="H8" s="0" t="s"/>
-      <x:c r="I8" s="0" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:9">
-      <x:c r="A9" s="0" t="s"/>
-      <x:c r="B9" s="0" t="s"/>
-      <x:c r="C9" s="0" t="s"/>
-      <x:c r="D9" s="0" t="s"/>
-      <x:c r="E9" s="0" t="s"/>
-      <x:c r="F9" s="0" t="s"/>
-      <x:c r="G9" s="0" t="s"/>
-      <x:c r="H9" s="0" t="s"/>
-      <x:c r="I9" s="0" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:9">
-      <x:c r="A10" s="0" t="s"/>
-      <x:c r="B10" s="0" t="s"/>
-      <x:c r="C10" s="0" t="s"/>
-      <x:c r="D10" s="0" t="s"/>
-      <x:c r="E10" s="0" t="s"/>
-      <x:c r="F10" s="0" t="s"/>
-      <x:c r="G10" s="0" t="s"/>
-      <x:c r="H10" s="0" t="s"/>
-      <x:c r="I10" s="0" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:9">
-      <x:c r="A11" s="0" t="s"/>
-      <x:c r="B11" s="0" t="s"/>
-      <x:c r="C11" s="0" t="s"/>
-      <x:c r="D11" s="0" t="s"/>
-      <x:c r="E11" s="0" t="s"/>
-      <x:c r="F11" s="0" t="s"/>
-      <x:c r="G11" s="0" t="s"/>
-      <x:c r="H11" s="0" t="s"/>
-      <x:c r="I11" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="9" spans="1:9"/>
+    <x:row r="10" spans="1:9"/>
+    <x:row r="11" spans="1:9"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1700,36 +1396,13 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:4"/>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="4" spans="1:4"/>
+    <x:row r="5" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1754,36 +1427,13 @@
     <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:4"/>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="4" spans="1:4"/>
+    <x:row r="5" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1810,40 +1460,16 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
     </x:row>
     <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="A6" s="0" t="s"/>
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="4" spans="1:4"/>
+    <x:row r="5" spans="1:4"/>
+    <x:row r="6" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1870,28 +1496,10 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="2" spans="1:4"/>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="4" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1916,41 +1524,15 @@
     <x:col min="1" max="5" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
-      <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-      <x:c r="E1" s="0" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:5"/>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-      <x:c r="E2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:5">
-      <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-      <x:c r="E3" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="3" spans="1:5"/>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-      <x:c r="E4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s"/>
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="5" spans="1:5"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -1977,28 +1559,10 @@
   <x:sheetData>
     <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-      <x:c r="C1" s="0" t="s"/>
-      <x:c r="D1" s="0" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-      <x:c r="C2" s="0" t="s"/>
-      <x:c r="D2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s"/>
-      <x:c r="B3" s="0" t="s"/>
-      <x:c r="C3" s="0" t="s"/>
-      <x:c r="D3" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
+    </x:row>
+    <x:row r="2" spans="1:4"/>
+    <x:row r="3" spans="1:4"/>
+    <x:row r="4" spans="1:4"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>